<commit_message>
a lot of stuff: start graphics tab and graphics backend, start contact tab and contact backend, add POST method to reset.js, modify tabs.js to expand tab selection when logo is clicked
</commit_message>
<xml_diff>
--- a/data/images.xlsx
+++ b/data/images.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="926" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>Filename</t>
   </si>
@@ -23,9 +23,6 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Copyright</t>
   </si>
   <si>
@@ -38,7 +35,7 @@
     <t>Dimensions</t>
   </si>
   <si>
-    <t>Duration</t>
+    <t>Orientation</t>
   </si>
   <si>
     <t>Hell Block.jpg</t>
@@ -47,7 +44,7 @@
     <t>Hell Block</t>
   </si>
   <si>
-    <t>&amp;copy; Alyssa Taylor</t>
+    <t>Alyssa Taylor</t>
   </si>
   <si>
     <t>Oil Paint on Canvas</t>
@@ -56,21 +53,27 @@
     <t>48"x36"</t>
   </si>
   <si>
+    <t>Landscape</t>
+  </si>
+  <si>
+    <t>Still Life in White #1.jpg</t>
+  </si>
+  <si>
+    <t>Still Life in White #1</t>
+  </si>
+  <si>
+    <t>18"x24"</t>
+  </si>
+  <si>
+    <t>Portrait</t>
+  </si>
+  <si>
     <t>Lucky #13.JPG</t>
   </si>
   <si>
     <t>Lucky #13</t>
   </si>
   <si>
-    <t>Still Life in White #1.jpg</t>
-  </si>
-  <si>
-    <t>Still Life in White #1</t>
-  </si>
-  <si>
-    <t>18"x24"</t>
-  </si>
-  <si>
     <t>Wisteria #1.JPG</t>
   </si>
   <si>
@@ -78,6 +81,12 @@
   </si>
   <si>
     <t>Synthetic Polymer on Canvas</t>
+  </si>
+  <si>
+    <t>Stella.jpg</t>
+  </si>
+  <si>
+    <t>Stella</t>
   </si>
 </sst>
 </file>
@@ -196,10 +205,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -207,7 +216,7 @@
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.4285714285714"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -229,23 +238,22 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>2013</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>2013</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>11</v>
@@ -253,7 +261,6 @@
       <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
@@ -262,54 +269,81 @@
       <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>2013</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="2" t="n">
-        <v>2015</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>2015</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>2013</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>2016</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>2016</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="2" t="n">
-        <v>2016</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>20</v>
+      <c r="G6" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove third party analytics, add my own analytics (thoughtful)
</commit_message>
<xml_diff>
--- a/data/images.xlsx
+++ b/data/images.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="926" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Filename</t>
   </si>
@@ -35,9 +35,6 @@
     <t>Dimensions</t>
   </si>
   <si>
-    <t>Orientation</t>
-  </si>
-  <si>
     <t>Hell Block.jpg</t>
   </si>
   <si>
@@ -53,9 +50,6 @@
     <t>48"x36"</t>
   </si>
   <si>
-    <t>Landscape</t>
-  </si>
-  <si>
     <t>Still Life in White #1.jpg</t>
   </si>
   <si>
@@ -65,9 +59,6 @@
     <t>18"x24"</t>
   </si>
   <si>
-    <t>Portrait</t>
-  </si>
-  <si>
     <t>Lucky #13.JPG</t>
   </si>
   <si>
@@ -83,7 +74,7 @@
     <t>Synthetic Polymer on Canvas</t>
   </si>
   <si>
-    <t>Stella.jpg</t>
+    <t>Still-Life in White #2.jpg</t>
   </si>
   <si>
     <t>Stella</t>
@@ -205,18 +196,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="7:11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.4285714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.984693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="14.4285714285714"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -235,117 +227,104 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>2013</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>2013</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>2015</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>2016</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>2016</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
add moile version, add library to handle swiping, mobile-ify gallery.js, add font-awesome for navbar bars, automatically detect mobile and redirect on client
</commit_message>
<xml_diff>
--- a/data/images.xlsx
+++ b/data/images.xlsx
@@ -1,12 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
@@ -106,7 +110,7 @@
     <t>16" x 20".</t>
   </si>
   <si>
-    <t>Still Life in White #2.jpg</t>
+    <t>Still-Life in White #2.jpg</t>
   </si>
   <si>
     <t>Still Life in White #2.</t>
@@ -142,7 +146,7 @@
     <t>14" x 11".</t>
   </si>
   <si>
-    <t>Redwood Picnic.jpeg</t>
+    <t>Redwood Picnic.jpg</t>
   </si>
   <si>
     <t>Redwood Picnic.</t>
@@ -154,20 +158,52 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
-    <font>
-      <sz val="10.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
+  </numFmts>
+  <fonts count="7">
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-    </font>
-    <font/>
-    <font>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -175,59 +211,96 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="0"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="14.4285714285714"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -247,7 +320,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -257,8 +330,8 @@
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2">
-        <v>2013.0</v>
+      <c r="D2" s="2" t="n">
+        <v>2013</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>9</v>
@@ -267,7 +340,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -277,8 +350,8 @@
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2">
-        <v>2013.0</v>
+      <c r="D3" s="2" t="n">
+        <v>2013</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>9</v>
@@ -287,7 +360,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -297,8 +370,8 @@
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2">
-        <v>2015.0</v>
+      <c r="D4" s="2" t="n">
+        <v>2015</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>9</v>
@@ -307,7 +380,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -317,8 +390,8 @@
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="2">
-        <v>2016.0</v>
+      <c r="D5" s="2" t="n">
+        <v>2016</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>19</v>
@@ -327,7 +400,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -337,8 +410,8 @@
       <c r="C6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2">
-        <v>2016.0</v>
+      <c r="D6" s="2" t="n">
+        <v>2016</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>23</v>
@@ -347,7 +420,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -357,8 +430,8 @@
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="2">
-        <v>2016.0</v>
+      <c r="D7" s="2" t="n">
+        <v>2016</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>9</v>
@@ -367,7 +440,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
@@ -377,8 +450,8 @@
       <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="2">
-        <v>2016.0</v>
+      <c r="D8" s="2" t="n">
+        <v>2016</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>19</v>
@@ -387,7 +460,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>31</v>
       </c>
@@ -397,8 +470,8 @@
       <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="2">
-        <v>2016.0</v>
+      <c r="D9" s="2" t="n">
+        <v>2016</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>9</v>
@@ -407,7 +480,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>33</v>
       </c>
@@ -417,8 +490,8 @@
       <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="2">
-        <v>2016.0</v>
+      <c r="D10" s="2" t="n">
+        <v>2016</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>35</v>
@@ -427,7 +500,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
@@ -437,8 +510,8 @@
       <c r="C11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="2">
-        <v>2014.0</v>
+      <c r="D11" s="2" t="n">
+        <v>2014</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
@@ -447,7 +520,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>39</v>
       </c>
@@ -457,8 +530,8 @@
       <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="2">
-        <v>2006.0</v>
+      <c r="D12" s="2" t="n">
+        <v>2006</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>41</v>
@@ -467,7 +540,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>43</v>
       </c>
@@ -477,8 +550,8 @@
       <c r="C13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="2">
-        <v>2013.0</v>
+      <c r="D13" s="2" t="n">
+        <v>2013</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>9</v>
@@ -488,6 +561,12 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>